<commit_message>
updates to calculae choropleth steps, cleaned data to catch muni code issues
</commit_message>
<xml_diff>
--- a/source files/burlington.xlsx
+++ b/source files/burlington.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Codes Docs\Guide to Affordable Hsg website tables\2022 tables\excel tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://etsorg1-my.sharepoint.com/personal/bgross_ets_org/Documents/ETS/misc/Pratt/semster 8/repo/affordable-housing-viz/source files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4421ECEC-3C39-4EAD-AFA9-C2C14F67C6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{4421ECEC-3C39-4EAD-AFA9-C2C14F67C6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA2492A3-8D31-4A72-9D9F-EFC35D84C4D6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F4C0807E-FF86-44D2-8965-0F9D93751DBD}"/>
   </bookViews>
@@ -4576,7 +4576,9 @@
   </sheetPr>
   <dimension ref="A1:AM274"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4589,18 +4591,20 @@
     <col min="8" max="8" width="3.85546875" customWidth="1"/>
     <col min="9" max="9" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="43.42578125" customWidth="1"/>
+    <col min="11" max="11" width="51" customWidth="1"/>
     <col min="12" max="13" width="9.140625" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="21.42578125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" hidden="1" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
+    <col min="21" max="21" width="18.42578125" customWidth="1"/>
     <col min="22" max="23" width="9.140625" customWidth="1"/>
     <col min="24" max="24" width="9.140625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" customWidth="1"/>
-    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="25.5703125" customWidth="1"/>
+    <col min="26" max="26" width="10.42578125" customWidth="1"/>
     <col min="29" max="29" width="54.140625" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="56.85546875" customWidth="1"/>

</xml_diff>